<commit_message>
Add the code - percentile rank, evaluation
</commit_message>
<xml_diff>
--- a/input/experiment_result.xlsx
+++ b/input/experiment_result.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\2360418_2_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D12F57A-A59B-439A-B949-A1BC0A07B464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="107">
   <si>
     <t>Block Type</t>
   </si>
@@ -195,33 +207,9 @@
     <t>Y</t>
   </si>
   <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>20230626_BC14</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>20230626_BC15</t>
-  </si>
-  <si>
     <t>Undetermined</t>
   </si>
   <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>20230626_BC19</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>DW</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -240,18 +228,6 @@
     <t>B5</t>
   </si>
   <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -270,18 +246,6 @@
     <t>C5</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -300,18 +264,6 @@
     <t>D5</t>
   </si>
   <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
     <t>E1</t>
   </si>
   <si>
@@ -330,18 +282,6 @@
     <t>E5</t>
   </si>
   <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -360,18 +300,6 @@
     <t>F5</t>
   </si>
   <si>
-    <t>F6</t>
-  </si>
-  <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>F9</t>
-  </si>
-  <si>
     <t>G1</t>
   </si>
   <si>
@@ -390,18 +318,6 @@
     <t>G5</t>
   </si>
   <si>
-    <t>G6</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>G8</t>
-  </si>
-  <si>
-    <t>G9</t>
-  </si>
-  <si>
     <t>H1</t>
   </si>
   <si>
@@ -418,18 +334,6 @@
   </si>
   <si>
     <t>H5</t>
-  </si>
-  <si>
-    <t>H6</t>
-  </si>
-  <si>
-    <t>H7</t>
-  </si>
-  <si>
-    <t>H8</t>
-  </si>
-  <si>
-    <t>H9</t>
   </si>
   <si>
     <t>Analysis Type</t>
@@ -453,7 +357,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -787,21 +691,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -817,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -825,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -833,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -841,7 +745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -849,7 +753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -941,7 +845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1035,15 +939,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -1129,15 +1033,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -1223,15 +1127,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -1317,15 +1221,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
@@ -1393,15 +1297,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
@@ -1469,15 +1373,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>
@@ -1563,15 +1467,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>45</v>
@@ -1654,7 +1558,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1746,15 +1650,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
@@ -1838,15 +1742,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>45</v>
@@ -1930,15 +1834,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
         <v>45</v>
@@ -2022,15 +1926,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
         <v>45</v>
@@ -2051,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K21" t="s">
         <v>11</v>
@@ -2114,15 +2018,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
         <v>45</v>
@@ -2206,15 +2110,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
         <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
@@ -2298,15 +2202,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
         <v>45</v>
@@ -2390,7 +2294,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2482,15 +2386,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>45</v>
@@ -2574,15 +2478,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>45</v>
@@ -2666,15 +2570,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
         <v>45</v>
@@ -2758,15 +2662,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>45</v>
@@ -2787,7 +2691,7 @@
         <v>11</v>
       </c>
       <c r="J29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -2850,15 +2754,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
         <v>45</v>
@@ -2879,7 +2783,7 @@
         <v>11</v>
       </c>
       <c r="J30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K30" t="s">
         <v>11</v>
@@ -2942,15 +2846,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
         <v>45</v>
@@ -3034,15 +2938,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
         <v>45</v>
@@ -3126,7 +3030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -3218,15 +3122,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>45</v>
@@ -3310,15 +3214,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
         <v>45</v>
@@ -3402,15 +3306,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
         <v>45</v>
@@ -3494,15 +3398,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
         <v>45</v>
@@ -3523,7 +3427,7 @@
         <v>11</v>
       </c>
       <c r="J37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K37" t="s">
         <v>11</v>
@@ -3586,15 +3490,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
         <v>45</v>
@@ -3615,7 +3519,7 @@
         <v>11</v>
       </c>
       <c r="J38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K38" t="s">
         <v>11</v>
@@ -3678,15 +3582,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
         <v>45</v>
@@ -3770,15 +3674,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
         <v>45</v>
@@ -3862,7 +3766,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -3954,15 +3858,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
         <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
         <v>45</v>
@@ -4046,15 +3950,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
         <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
@@ -4138,15 +4042,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
         <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
         <v>45</v>
@@ -4230,15 +4134,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
         <v>45</v>
@@ -4322,15 +4226,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
         <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
         <v>45</v>
@@ -4351,7 +4255,7 @@
         <v>11</v>
       </c>
       <c r="J46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K46" t="s">
         <v>11</v>
@@ -4414,15 +4318,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D47" t="s">
         <v>45</v>
@@ -4506,15 +4410,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
         <v>45</v>
@@ -4598,2979 +4502,35 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D49" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" t="s">
-        <v>47</v>
-      </c>
-      <c r="G49" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" t="s">
-        <v>11</v>
-      </c>
-      <c r="I49" t="s">
-        <v>11</v>
-      </c>
-      <c r="J49">
-        <v>25.957450866699219</v>
-      </c>
-      <c r="K49">
-        <v>25.957450866699219</v>
-      </c>
-      <c r="L49" t="s">
-        <v>11</v>
-      </c>
-      <c r="M49" t="s">
-        <v>11</v>
-      </c>
-      <c r="N49" t="s">
-        <v>11</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P49" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>11</v>
-      </c>
-      <c r="R49" t="s">
-        <v>11</v>
-      </c>
-      <c r="S49" t="b">
-        <v>1</v>
-      </c>
-      <c r="T49">
-        <v>8792.2417853860297</v>
-      </c>
-      <c r="U49" t="b">
-        <v>1</v>
-      </c>
-      <c r="V49">
-        <v>3</v>
-      </c>
-      <c r="W49">
-        <v>19</v>
-      </c>
-      <c r="X49">
-        <v>1</v>
-      </c>
-      <c r="Y49">
-        <v>87.8375244140625</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB49" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" t="s">
-        <v>47</v>
-      </c>
-      <c r="G50" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" t="s">
-        <v>11</v>
-      </c>
-      <c r="J50">
-        <v>25.526128768920898</v>
-      </c>
-      <c r="K50">
-        <v>25.526128768920898</v>
-      </c>
-      <c r="L50" t="s">
-        <v>11</v>
-      </c>
-      <c r="M50" t="s">
-        <v>11</v>
-      </c>
-      <c r="N50" t="s">
-        <v>11</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P50" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>11</v>
-      </c>
-      <c r="R50" t="s">
-        <v>11</v>
-      </c>
-      <c r="S50" t="b">
-        <v>1</v>
-      </c>
-      <c r="T50">
-        <v>7903.1422125153931</v>
-      </c>
-      <c r="U50" t="b">
-        <v>1</v>
-      </c>
-      <c r="V50">
-        <v>3</v>
-      </c>
-      <c r="W50">
-        <v>19</v>
-      </c>
-      <c r="X50">
-        <v>1</v>
-      </c>
-      <c r="Y50">
-        <v>87.8375244140625</v>
-      </c>
-      <c r="Z50" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA50" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB50" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC50" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" t="s">
-        <v>78</v>
-      </c>
-      <c r="D51" t="s">
-        <v>45</v>
-      </c>
-      <c r="E51" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" t="s">
-        <v>47</v>
-      </c>
-      <c r="G51" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" t="s">
-        <v>11</v>
-      </c>
-      <c r="J51">
-        <v>22.943403244018555</v>
-      </c>
-      <c r="K51">
-        <v>22.943403244018555</v>
-      </c>
-      <c r="L51" t="s">
-        <v>11</v>
-      </c>
-      <c r="M51" t="s">
-        <v>11</v>
-      </c>
-      <c r="N51" t="s">
-        <v>11</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P51" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>11</v>
-      </c>
-      <c r="R51" t="s">
-        <v>11</v>
-      </c>
-      <c r="S51" t="b">
-        <v>1</v>
-      </c>
-      <c r="T51">
-        <v>11856.551798592032</v>
-      </c>
-      <c r="U51" t="b">
-        <v>1</v>
-      </c>
-      <c r="V51">
-        <v>3</v>
-      </c>
-      <c r="W51">
-        <v>16</v>
-      </c>
-      <c r="X51">
-        <v>1</v>
-      </c>
-      <c r="Y51">
-        <v>87.8375244140625</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA51" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB51" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC51" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" t="s">
-        <v>45</v>
-      </c>
-      <c r="E52" t="s">
-        <v>46</v>
-      </c>
-      <c r="F52" t="s">
-        <v>47</v>
-      </c>
-      <c r="G52" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" t="s">
-        <v>11</v>
-      </c>
-      <c r="I52" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52">
-        <v>21.552255630493164</v>
-      </c>
-      <c r="K52">
-        <v>21.552255630493164</v>
-      </c>
-      <c r="L52" t="s">
-        <v>11</v>
-      </c>
-      <c r="M52" t="s">
-        <v>11</v>
-      </c>
-      <c r="N52" t="s">
-        <v>11</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P52" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>11</v>
-      </c>
-      <c r="R52" t="s">
-        <v>11</v>
-      </c>
-      <c r="S52" t="b">
-        <v>1</v>
-      </c>
-      <c r="T52">
-        <v>2446.3801850145992</v>
-      </c>
-      <c r="U52" t="b">
-        <v>1</v>
-      </c>
-      <c r="V52">
-        <v>3</v>
-      </c>
-      <c r="W52">
-        <v>15</v>
-      </c>
-      <c r="X52">
-        <v>1</v>
-      </c>
-      <c r="Y52">
-        <v>87.638702392578125</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA52" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB52" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC52" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" t="s">
-        <v>98</v>
-      </c>
-      <c r="D53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" t="s">
-        <v>47</v>
-      </c>
-      <c r="G53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I53" t="s">
-        <v>11</v>
-      </c>
-      <c r="J53">
-        <v>19.852371215820313</v>
-      </c>
-      <c r="K53">
-        <v>19.852371215820313</v>
-      </c>
-      <c r="L53" t="s">
-        <v>11</v>
-      </c>
-      <c r="M53" t="s">
-        <v>11</v>
-      </c>
-      <c r="N53" t="s">
-        <v>11</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P53" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>11</v>
-      </c>
-      <c r="R53" t="s">
-        <v>11</v>
-      </c>
-      <c r="S53" t="b">
-        <v>1</v>
-      </c>
-      <c r="T53">
-        <v>453.9028514530811</v>
-      </c>
-      <c r="U53" t="b">
-        <v>1</v>
-      </c>
-      <c r="V53">
-        <v>3</v>
-      </c>
-      <c r="W53">
-        <v>18</v>
-      </c>
-      <c r="X53">
-        <v>1</v>
-      </c>
-      <c r="Y53">
-        <v>87.8375244140625</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA53" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB53" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC53" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" t="s">
-        <v>45</v>
-      </c>
-      <c r="E54" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" t="s">
-        <v>47</v>
-      </c>
-      <c r="G54" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" t="s">
-        <v>11</v>
-      </c>
-      <c r="I54" t="s">
-        <v>11</v>
-      </c>
-      <c r="J54" t="s">
-        <v>62</v>
-      </c>
-      <c r="K54" t="s">
-        <v>11</v>
-      </c>
-      <c r="L54" t="s">
-        <v>11</v>
-      </c>
-      <c r="M54" t="s">
-        <v>11</v>
-      </c>
-      <c r="N54" t="s">
-        <v>11</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P54" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>11</v>
-      </c>
-      <c r="R54" t="s">
-        <v>11</v>
-      </c>
-      <c r="S54" t="b">
-        <v>1</v>
-      </c>
-      <c r="T54">
-        <v>949.45575971407459</v>
-      </c>
-      <c r="U54" t="b">
-        <v>1</v>
-      </c>
-      <c r="V54">
-        <v>3</v>
-      </c>
-      <c r="W54">
-        <v>39</v>
-      </c>
-      <c r="X54">
-        <v>1</v>
-      </c>
-      <c r="Y54">
-        <v>61.792926788330078</v>
-      </c>
-      <c r="Z54" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA54" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB54" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC54" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>123</v>
-      </c>
-      <c r="B55" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
-      </c>
-      <c r="D55" t="s">
-        <v>45</v>
-      </c>
-      <c r="E55" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" t="s">
-        <v>47</v>
-      </c>
-      <c r="G55" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" t="s">
-        <v>11</v>
-      </c>
-      <c r="I55" t="s">
-        <v>11</v>
-      </c>
-      <c r="J55" t="s">
-        <v>62</v>
-      </c>
-      <c r="K55" t="s">
-        <v>11</v>
-      </c>
-      <c r="L55" t="s">
-        <v>11</v>
-      </c>
-      <c r="M55" t="s">
-        <v>11</v>
-      </c>
-      <c r="N55" t="s">
-        <v>11</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P55" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>11</v>
-      </c>
-      <c r="R55" t="s">
-        <v>11</v>
-      </c>
-      <c r="S55" t="b">
-        <v>1</v>
-      </c>
-      <c r="T55">
-        <v>8859.4800092846945</v>
-      </c>
-      <c r="U55" t="b">
-        <v>1</v>
-      </c>
-      <c r="V55">
-        <v>3</v>
-      </c>
-      <c r="W55">
-        <v>39</v>
-      </c>
-      <c r="X55">
-        <v>1</v>
-      </c>
-      <c r="Y55">
-        <v>61.594112396240234</v>
-      </c>
-      <c r="Z55" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA55" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB55" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC55" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" t="s">
-        <v>45</v>
-      </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" t="s">
-        <v>11</v>
-      </c>
-      <c r="J56" t="s">
-        <v>62</v>
-      </c>
-      <c r="K56" t="s">
-        <v>11</v>
-      </c>
-      <c r="L56" t="s">
-        <v>11</v>
-      </c>
-      <c r="M56" t="s">
-        <v>11</v>
-      </c>
-      <c r="N56" t="s">
-        <v>11</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P56" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>11</v>
-      </c>
-      <c r="R56" t="s">
-        <v>11</v>
-      </c>
-      <c r="S56" t="b">
-        <v>1</v>
-      </c>
-      <c r="T56">
-        <v>20991.264453125001</v>
-      </c>
-      <c r="U56" t="b">
-        <v>1</v>
-      </c>
-      <c r="V56">
-        <v>3</v>
-      </c>
-      <c r="W56">
-        <v>38</v>
-      </c>
-      <c r="X56">
-        <v>1</v>
-      </c>
-      <c r="Y56">
-        <v>61.395298004150391</v>
-      </c>
-      <c r="Z56" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA56" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB56" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC56" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" t="s">
-        <v>61</v>
-      </c>
-      <c r="C57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E57" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" t="s">
-        <v>11</v>
-      </c>
-      <c r="I57" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" t="s">
-        <v>62</v>
-      </c>
-      <c r="K57" t="s">
-        <v>11</v>
-      </c>
-      <c r="L57" t="s">
-        <v>11</v>
-      </c>
-      <c r="M57" t="s">
-        <v>11</v>
-      </c>
-      <c r="N57" t="s">
-        <v>11</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P57" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>11</v>
-      </c>
-      <c r="R57" t="s">
-        <v>11</v>
-      </c>
-      <c r="S57" t="b">
-        <v>1</v>
-      </c>
-      <c r="T57">
-        <v>8792.2417853860297</v>
-      </c>
-      <c r="U57" t="b">
-        <v>1</v>
-      </c>
-      <c r="V57">
-        <v>3</v>
-      </c>
-      <c r="W57">
-        <v>38</v>
-      </c>
-      <c r="X57">
-        <v>1</v>
-      </c>
-      <c r="Y57">
-        <v>64.971588134765625</v>
-      </c>
-      <c r="Z57" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB57" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC57" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" t="s">
-        <v>47</v>
-      </c>
-      <c r="G58" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" t="s">
-        <v>11</v>
-      </c>
-      <c r="I58" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" t="s">
-        <v>62</v>
-      </c>
-      <c r="K58" t="s">
-        <v>11</v>
-      </c>
-      <c r="L58" t="s">
-        <v>11</v>
-      </c>
-      <c r="M58" t="s">
-        <v>11</v>
-      </c>
-      <c r="N58" t="s">
-        <v>11</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P58" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>11</v>
-      </c>
-      <c r="R58" t="s">
-        <v>11</v>
-      </c>
-      <c r="S58" t="b">
-        <v>1</v>
-      </c>
-      <c r="T58">
-        <v>7903.1422125153931</v>
-      </c>
-      <c r="U58" t="b">
-        <v>1</v>
-      </c>
-      <c r="V58">
-        <v>3</v>
-      </c>
-      <c r="W58">
-        <v>29</v>
-      </c>
-      <c r="X58">
-        <v>1</v>
-      </c>
-      <c r="Y58">
-        <v>70.340034484863281</v>
-      </c>
-      <c r="Z58" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA58" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB58" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC58" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" t="s">
-        <v>78</v>
-      </c>
-      <c r="D59" t="s">
-        <v>45</v>
-      </c>
-      <c r="E59" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" t="s">
-        <v>47</v>
-      </c>
-      <c r="G59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" t="s">
-        <v>11</v>
-      </c>
-      <c r="I59" t="s">
-        <v>11</v>
-      </c>
-      <c r="J59" t="s">
-        <v>62</v>
-      </c>
-      <c r="K59" t="s">
-        <v>11</v>
-      </c>
-      <c r="L59" t="s">
-        <v>11</v>
-      </c>
-      <c r="M59" t="s">
-        <v>11</v>
-      </c>
-      <c r="N59" t="s">
-        <v>11</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P59" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>11</v>
-      </c>
-      <c r="R59" t="s">
-        <v>11</v>
-      </c>
-      <c r="S59" t="b">
-        <v>1</v>
-      </c>
-      <c r="T59">
-        <v>11856.551798592032</v>
-      </c>
-      <c r="U59" t="b">
-        <v>1</v>
-      </c>
-      <c r="V59">
-        <v>3</v>
-      </c>
-      <c r="W59">
-        <v>38</v>
-      </c>
-      <c r="X59">
-        <v>1</v>
-      </c>
-      <c r="Y59">
-        <v>61.392620086669922</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA59" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB59" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC59" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD59" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" t="s">
-        <v>88</v>
-      </c>
-      <c r="D60" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G60" t="s">
-        <v>11</v>
-      </c>
-      <c r="H60" t="s">
-        <v>11</v>
-      </c>
-      <c r="I60" t="s">
-        <v>11</v>
-      </c>
-      <c r="J60" t="s">
-        <v>62</v>
-      </c>
-      <c r="K60" t="s">
-        <v>11</v>
-      </c>
-      <c r="L60" t="s">
-        <v>11</v>
-      </c>
-      <c r="M60" t="s">
-        <v>11</v>
-      </c>
-      <c r="N60" t="s">
-        <v>11</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P60" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>11</v>
-      </c>
-      <c r="R60" t="s">
-        <v>11</v>
-      </c>
-      <c r="S60" t="b">
-        <v>1</v>
-      </c>
-      <c r="T60">
-        <v>2446.3801850145992</v>
-      </c>
-      <c r="U60" t="b">
-        <v>1</v>
-      </c>
-      <c r="V60">
-        <v>3</v>
-      </c>
-      <c r="W60">
-        <v>18</v>
-      </c>
-      <c r="X60">
-        <v>1</v>
-      </c>
-      <c r="Y60">
-        <v>61.790283203125</v>
-      </c>
-      <c r="Z60" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA60" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB60" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC60" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" t="s">
-        <v>45</v>
-      </c>
-      <c r="E61" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" t="s">
-        <v>47</v>
-      </c>
-      <c r="G61" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" t="s">
-        <v>11</v>
-      </c>
-      <c r="I61" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61" t="s">
-        <v>62</v>
-      </c>
-      <c r="K61" t="s">
-        <v>11</v>
-      </c>
-      <c r="L61" t="s">
-        <v>11</v>
-      </c>
-      <c r="M61" t="s">
-        <v>11</v>
-      </c>
-      <c r="N61" t="s">
-        <v>11</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P61" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>11</v>
-      </c>
-      <c r="R61" t="s">
-        <v>11</v>
-      </c>
-      <c r="S61" t="b">
-        <v>1</v>
-      </c>
-      <c r="T61">
-        <v>453.9028514530811</v>
-      </c>
-      <c r="U61" t="b">
-        <v>1</v>
-      </c>
-      <c r="V61">
-        <v>3</v>
-      </c>
-      <c r="W61">
-        <v>37</v>
-      </c>
-      <c r="X61">
-        <v>1</v>
-      </c>
-      <c r="Y61">
-        <v>66.562240600585938</v>
-      </c>
-      <c r="Z61" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB61" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC61" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD61" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" t="s">
-        <v>108</v>
-      </c>
-      <c r="D62" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" t="s">
-        <v>47</v>
-      </c>
-      <c r="G62" t="s">
-        <v>11</v>
-      </c>
-      <c r="H62" t="s">
-        <v>11</v>
-      </c>
-      <c r="I62" t="s">
-        <v>11</v>
-      </c>
-      <c r="J62" t="s">
-        <v>62</v>
-      </c>
-      <c r="K62" t="s">
-        <v>11</v>
-      </c>
-      <c r="L62" t="s">
-        <v>11</v>
-      </c>
-      <c r="M62" t="s">
-        <v>11</v>
-      </c>
-      <c r="N62" t="s">
-        <v>11</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P62" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>11</v>
-      </c>
-      <c r="R62" t="s">
-        <v>11</v>
-      </c>
-      <c r="S62" t="b">
-        <v>1</v>
-      </c>
-      <c r="T62">
-        <v>949.45575971407459</v>
-      </c>
-      <c r="U62" t="b">
-        <v>1</v>
-      </c>
-      <c r="V62">
-        <v>1</v>
-      </c>
-      <c r="W62">
-        <v>2</v>
-      </c>
-      <c r="X62">
-        <v>1</v>
-      </c>
-      <c r="Y62">
-        <v>72.328353881835938</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA62" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB62" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC62" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD62" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
-      <c r="C63" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" t="s">
-        <v>45</v>
-      </c>
-      <c r="E63" t="s">
-        <v>46</v>
-      </c>
-      <c r="F63" t="s">
-        <v>47</v>
-      </c>
-      <c r="G63" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" t="s">
-        <v>11</v>
-      </c>
-      <c r="J63" t="s">
-        <v>62</v>
-      </c>
-      <c r="K63" t="s">
-        <v>11</v>
-      </c>
-      <c r="L63" t="s">
-        <v>11</v>
-      </c>
-      <c r="M63" t="s">
-        <v>11</v>
-      </c>
-      <c r="N63" t="s">
-        <v>11</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P63" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>11</v>
-      </c>
-      <c r="R63" t="s">
-        <v>11</v>
-      </c>
-      <c r="S63" t="b">
-        <v>1</v>
-      </c>
-      <c r="T63">
-        <v>8859.4800092846945</v>
-      </c>
-      <c r="U63" t="b">
-        <v>1</v>
-      </c>
-      <c r="V63">
-        <v>3</v>
-      </c>
-      <c r="W63">
-        <v>36</v>
-      </c>
-      <c r="X63">
-        <v>1</v>
-      </c>
-      <c r="Y63">
-        <v>70.538864135742188</v>
-      </c>
-      <c r="Z63" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA63" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB63" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC63" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD63" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>134</v>
-      </c>
-      <c r="B64" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" t="s">
-        <v>45</v>
-      </c>
-      <c r="E64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F64" t="s">
-        <v>47</v>
-      </c>
-      <c r="G64" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" t="s">
-        <v>11</v>
-      </c>
-      <c r="J64" t="s">
-        <v>62</v>
-      </c>
-      <c r="K64" t="s">
-        <v>11</v>
-      </c>
-      <c r="L64" t="s">
-        <v>11</v>
-      </c>
-      <c r="M64" t="s">
-        <v>11</v>
-      </c>
-      <c r="N64" t="s">
-        <v>11</v>
-      </c>
-      <c r="O64" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P64" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>11</v>
-      </c>
-      <c r="R64" t="s">
-        <v>11</v>
-      </c>
-      <c r="S64" t="b">
-        <v>1</v>
-      </c>
-      <c r="T64">
-        <v>20991.264453125001</v>
-      </c>
-      <c r="U64" t="b">
-        <v>1</v>
-      </c>
-      <c r="V64">
-        <v>3</v>
-      </c>
-      <c r="W64">
-        <v>38</v>
-      </c>
-      <c r="X64">
-        <v>1</v>
-      </c>
-      <c r="Y64">
-        <v>91.813827514648438</v>
-      </c>
-      <c r="Z64">
-        <v>86.843048095703125</v>
-      </c>
-      <c r="AA64">
-        <v>64.176261901855469</v>
-      </c>
-      <c r="AB64" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC64" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD64" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D65" t="s">
-        <v>45</v>
-      </c>
-      <c r="E65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F65" t="s">
-        <v>47</v>
-      </c>
-      <c r="G65" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" t="s">
-        <v>11</v>
-      </c>
-      <c r="J65" t="s">
-        <v>62</v>
-      </c>
-      <c r="K65" t="s">
-        <v>11</v>
-      </c>
-      <c r="L65" t="s">
-        <v>11</v>
-      </c>
-      <c r="M65" t="s">
-        <v>11</v>
-      </c>
-      <c r="N65" t="s">
-        <v>11</v>
-      </c>
-      <c r="O65" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P65" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>11</v>
-      </c>
-      <c r="R65" t="s">
-        <v>11</v>
-      </c>
-      <c r="S65" t="b">
-        <v>1</v>
-      </c>
-      <c r="T65">
-        <v>8792.2417853860297</v>
-      </c>
-      <c r="U65" t="b">
-        <v>1</v>
-      </c>
-      <c r="V65">
-        <v>3</v>
-      </c>
-      <c r="W65">
-        <v>13</v>
-      </c>
-      <c r="X65">
-        <v>1</v>
-      </c>
-      <c r="Y65">
-        <v>61.392620086669922</v>
-      </c>
-      <c r="Z65" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA65" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB65" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC65" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" t="s">
-        <v>45</v>
-      </c>
-      <c r="E66" t="s">
-        <v>46</v>
-      </c>
-      <c r="F66" t="s">
-        <v>47</v>
-      </c>
-      <c r="G66" t="s">
-        <v>11</v>
-      </c>
-      <c r="H66" t="s">
-        <v>11</v>
-      </c>
-      <c r="I66" t="s">
-        <v>11</v>
-      </c>
-      <c r="J66" t="s">
-        <v>62</v>
-      </c>
-      <c r="K66" t="s">
-        <v>11</v>
-      </c>
-      <c r="L66" t="s">
-        <v>11</v>
-      </c>
-      <c r="M66" t="s">
-        <v>11</v>
-      </c>
-      <c r="N66" t="s">
-        <v>11</v>
-      </c>
-      <c r="O66" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P66" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>11</v>
-      </c>
-      <c r="R66" t="s">
-        <v>11</v>
-      </c>
-      <c r="S66" t="b">
-        <v>1</v>
-      </c>
-      <c r="T66">
-        <v>7903.1422125153931</v>
-      </c>
-      <c r="U66" t="b">
-        <v>1</v>
-      </c>
-      <c r="V66">
-        <v>3</v>
-      </c>
-      <c r="W66">
-        <v>38</v>
-      </c>
-      <c r="X66">
-        <v>1</v>
-      </c>
-      <c r="Y66">
-        <v>60.796127319335938</v>
-      </c>
-      <c r="Z66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC66" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B67" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" t="s">
-        <v>45</v>
-      </c>
-      <c r="E67" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" t="s">
-        <v>47</v>
-      </c>
-      <c r="G67" t="s">
-        <v>11</v>
-      </c>
-      <c r="H67" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67" t="s">
-        <v>11</v>
-      </c>
-      <c r="J67" t="s">
-        <v>62</v>
-      </c>
-      <c r="K67" t="s">
-        <v>11</v>
-      </c>
-      <c r="L67" t="s">
-        <v>11</v>
-      </c>
-      <c r="M67" t="s">
-        <v>11</v>
-      </c>
-      <c r="N67" t="s">
-        <v>11</v>
-      </c>
-      <c r="O67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P67" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>11</v>
-      </c>
-      <c r="R67" t="s">
-        <v>11</v>
-      </c>
-      <c r="S67" t="b">
-        <v>1</v>
-      </c>
-      <c r="T67">
-        <v>11856.551798592032</v>
-      </c>
-      <c r="U67" t="b">
-        <v>1</v>
-      </c>
-      <c r="V67">
-        <v>3</v>
-      </c>
-      <c r="W67">
-        <v>38</v>
-      </c>
-      <c r="X67">
-        <v>1</v>
-      </c>
-      <c r="Y67">
-        <v>60.597297668457031</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA67" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB67" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC67" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD67" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" t="s">
-        <v>88</v>
-      </c>
-      <c r="D68" t="s">
-        <v>45</v>
-      </c>
-      <c r="E68" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" t="s">
-        <v>47</v>
-      </c>
-      <c r="G68" t="s">
-        <v>11</v>
-      </c>
-      <c r="H68" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68" t="s">
-        <v>11</v>
-      </c>
-      <c r="J68" t="s">
-        <v>62</v>
-      </c>
-      <c r="K68" t="s">
-        <v>11</v>
-      </c>
-      <c r="L68" t="s">
-        <v>11</v>
-      </c>
-      <c r="M68" t="s">
-        <v>11</v>
-      </c>
-      <c r="N68" t="s">
-        <v>11</v>
-      </c>
-      <c r="O68" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P68" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>11</v>
-      </c>
-      <c r="R68" t="s">
-        <v>11</v>
-      </c>
-      <c r="S68" t="b">
-        <v>1</v>
-      </c>
-      <c r="T68">
-        <v>2446.3801850145992</v>
-      </c>
-      <c r="U68" t="b">
-        <v>1</v>
-      </c>
-      <c r="V68">
-        <v>3</v>
-      </c>
-      <c r="W68">
-        <v>5</v>
-      </c>
-      <c r="X68">
-        <v>1</v>
-      </c>
-      <c r="Y68">
-        <v>63.579765319824219</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA68" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB68" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC68" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" t="s">
-        <v>98</v>
-      </c>
-      <c r="D69" t="s">
-        <v>45</v>
-      </c>
-      <c r="E69" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" t="s">
-        <v>47</v>
-      </c>
-      <c r="G69" t="s">
-        <v>11</v>
-      </c>
-      <c r="H69" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" t="s">
-        <v>11</v>
-      </c>
-      <c r="J69" t="s">
-        <v>62</v>
-      </c>
-      <c r="K69" t="s">
-        <v>11</v>
-      </c>
-      <c r="L69" t="s">
-        <v>11</v>
-      </c>
-      <c r="M69" t="s">
-        <v>11</v>
-      </c>
-      <c r="N69" t="s">
-        <v>11</v>
-      </c>
-      <c r="O69" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P69" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>11</v>
-      </c>
-      <c r="R69" t="s">
-        <v>11</v>
-      </c>
-      <c r="S69" t="b">
-        <v>1</v>
-      </c>
-      <c r="T69">
-        <v>453.9028514530811</v>
-      </c>
-      <c r="U69" t="b">
-        <v>1</v>
-      </c>
-      <c r="V69">
-        <v>3</v>
-      </c>
-      <c r="W69">
-        <v>17</v>
-      </c>
-      <c r="X69">
-        <v>1</v>
-      </c>
-      <c r="Y69">
-        <v>63.778598785400391</v>
-      </c>
-      <c r="Z69" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA69" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB69" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC69" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD69" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>115</v>
-      </c>
-      <c r="B70" t="s">
-        <v>64</v>
-      </c>
-      <c r="C70" t="s">
-        <v>108</v>
-      </c>
-      <c r="D70" t="s">
-        <v>45</v>
-      </c>
-      <c r="E70" t="s">
-        <v>46</v>
-      </c>
-      <c r="F70" t="s">
-        <v>47</v>
-      </c>
-      <c r="G70" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" t="s">
-        <v>11</v>
-      </c>
-      <c r="I70" t="s">
-        <v>11</v>
-      </c>
-      <c r="J70" t="s">
-        <v>62</v>
-      </c>
-      <c r="K70" t="s">
-        <v>11</v>
-      </c>
-      <c r="L70" t="s">
-        <v>11</v>
-      </c>
-      <c r="M70" t="s">
-        <v>11</v>
-      </c>
-      <c r="N70" t="s">
-        <v>11</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P70" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>11</v>
-      </c>
-      <c r="R70" t="s">
-        <v>11</v>
-      </c>
-      <c r="S70" t="b">
-        <v>1</v>
-      </c>
-      <c r="T70">
-        <v>949.45575971407459</v>
-      </c>
-      <c r="U70" t="b">
-        <v>1</v>
-      </c>
-      <c r="V70">
-        <v>3</v>
-      </c>
-      <c r="W70">
-        <v>38</v>
-      </c>
-      <c r="X70">
-        <v>1</v>
-      </c>
-      <c r="Y70">
-        <v>60.796127319335938</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA70" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB70" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC70" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD70" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>125</v>
-      </c>
-      <c r="B71" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" t="s">
-        <v>118</v>
-      </c>
-      <c r="D71" t="s">
-        <v>45</v>
-      </c>
-      <c r="E71" t="s">
-        <v>46</v>
-      </c>
-      <c r="F71" t="s">
-        <v>47</v>
-      </c>
-      <c r="G71" t="s">
-        <v>11</v>
-      </c>
-      <c r="H71" t="s">
-        <v>11</v>
-      </c>
-      <c r="I71" t="s">
-        <v>11</v>
-      </c>
-      <c r="J71" t="s">
-        <v>62</v>
-      </c>
-      <c r="K71" t="s">
-        <v>11</v>
-      </c>
-      <c r="L71" t="s">
-        <v>11</v>
-      </c>
-      <c r="M71" t="s">
-        <v>11</v>
-      </c>
-      <c r="N71" t="s">
-        <v>11</v>
-      </c>
-      <c r="O71" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P71" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>11</v>
-      </c>
-      <c r="R71" t="s">
-        <v>11</v>
-      </c>
-      <c r="S71" t="b">
-        <v>1</v>
-      </c>
-      <c r="T71">
-        <v>8859.4800092846945</v>
-      </c>
-      <c r="U71" t="b">
-        <v>1</v>
-      </c>
-      <c r="V71">
-        <v>3</v>
-      </c>
-      <c r="W71">
-        <v>21</v>
-      </c>
-      <c r="X71">
-        <v>1</v>
-      </c>
-      <c r="Y71">
-        <v>61.989116668701172</v>
-      </c>
-      <c r="Z71" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA71" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB71" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC71" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD71" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>135</v>
-      </c>
-      <c r="B72" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72" t="s">
-        <v>45</v>
-      </c>
-      <c r="E72" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" t="s">
-        <v>47</v>
-      </c>
-      <c r="G72" t="s">
-        <v>11</v>
-      </c>
-      <c r="H72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I72" t="s">
-        <v>11</v>
-      </c>
-      <c r="J72" t="s">
-        <v>62</v>
-      </c>
-      <c r="K72" t="s">
-        <v>11</v>
-      </c>
-      <c r="L72" t="s">
-        <v>11</v>
-      </c>
-      <c r="M72" t="s">
-        <v>11</v>
-      </c>
-      <c r="N72" t="s">
-        <v>11</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P72" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>11</v>
-      </c>
-      <c r="R72" t="s">
-        <v>11</v>
-      </c>
-      <c r="S72" t="b">
-        <v>1</v>
-      </c>
-      <c r="T72">
-        <v>20991.264453125001</v>
-      </c>
-      <c r="U72" t="b">
-        <v>1</v>
-      </c>
-      <c r="V72">
-        <v>3</v>
-      </c>
-      <c r="W72">
-        <v>37</v>
-      </c>
-      <c r="X72">
-        <v>1</v>
-      </c>
-      <c r="Y72">
-        <v>70.538864135742188</v>
-      </c>
-      <c r="Z72">
-        <v>80.082778930664063</v>
-      </c>
-      <c r="AA72">
-        <v>61.790283203125</v>
-      </c>
-      <c r="AB72" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC72" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD72" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" t="s">
-        <v>44</v>
-      </c>
-      <c r="D73" t="s">
-        <v>45</v>
-      </c>
-      <c r="E73" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" t="s">
-        <v>47</v>
-      </c>
-      <c r="G73" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" t="s">
-        <v>11</v>
-      </c>
-      <c r="I73" t="s">
-        <v>11</v>
-      </c>
-      <c r="J73" t="s">
-        <v>62</v>
-      </c>
-      <c r="K73" t="s">
-        <v>11</v>
-      </c>
-      <c r="L73" t="s">
-        <v>11</v>
-      </c>
-      <c r="M73" t="s">
-        <v>11</v>
-      </c>
-      <c r="N73" t="s">
-        <v>11</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P73" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>11</v>
-      </c>
-      <c r="R73" t="s">
-        <v>11</v>
-      </c>
-      <c r="S73" t="b">
-        <v>1</v>
-      </c>
-      <c r="T73">
-        <v>8792.2417853860297</v>
-      </c>
-      <c r="U73" t="b">
-        <v>1</v>
-      </c>
-      <c r="V73">
-        <v>3</v>
-      </c>
-      <c r="W73">
-        <v>11</v>
-      </c>
-      <c r="X73">
-        <v>1</v>
-      </c>
-      <c r="Y73">
-        <v>65.969253540039063</v>
-      </c>
-      <c r="Z73" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA73" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB73" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC73" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>76</v>
-      </c>
-      <c r="B74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C74" t="s">
-        <v>68</v>
-      </c>
-      <c r="D74" t="s">
-        <v>45</v>
-      </c>
-      <c r="E74" t="s">
-        <v>46</v>
-      </c>
-      <c r="F74" t="s">
-        <v>47</v>
-      </c>
-      <c r="G74" t="s">
-        <v>11</v>
-      </c>
-      <c r="H74" t="s">
-        <v>11</v>
-      </c>
-      <c r="I74" t="s">
-        <v>11</v>
-      </c>
-      <c r="J74" t="s">
-        <v>62</v>
-      </c>
-      <c r="K74" t="s">
-        <v>11</v>
-      </c>
-      <c r="L74" t="s">
-        <v>11</v>
-      </c>
-      <c r="M74" t="s">
-        <v>11</v>
-      </c>
-      <c r="N74" t="s">
-        <v>11</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P74" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>11</v>
-      </c>
-      <c r="R74" t="s">
-        <v>11</v>
-      </c>
-      <c r="S74" t="b">
-        <v>1</v>
-      </c>
-      <c r="T74">
-        <v>7903.1422125153931</v>
-      </c>
-      <c r="U74" t="b">
-        <v>1</v>
-      </c>
-      <c r="V74">
-        <v>3</v>
-      </c>
-      <c r="W74">
-        <v>8</v>
-      </c>
-      <c r="X74">
-        <v>1</v>
-      </c>
-      <c r="Y74">
-        <v>63.384567260742188</v>
-      </c>
-      <c r="Z74" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA74" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB74" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC74" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>86</v>
-      </c>
-      <c r="B75" t="s">
-        <v>66</v>
-      </c>
-      <c r="C75" t="s">
-        <v>78</v>
-      </c>
-      <c r="D75" t="s">
-        <v>45</v>
-      </c>
-      <c r="E75" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" t="s">
-        <v>47</v>
-      </c>
-      <c r="G75" t="s">
-        <v>11</v>
-      </c>
-      <c r="H75" t="s">
-        <v>11</v>
-      </c>
-      <c r="I75" t="s">
-        <v>11</v>
-      </c>
-      <c r="J75" t="s">
-        <v>62</v>
-      </c>
-      <c r="K75" t="s">
-        <v>11</v>
-      </c>
-      <c r="L75" t="s">
-        <v>11</v>
-      </c>
-      <c r="M75" t="s">
-        <v>11</v>
-      </c>
-      <c r="N75" t="s">
-        <v>11</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P75" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>11</v>
-      </c>
-      <c r="R75" t="s">
-        <v>11</v>
-      </c>
-      <c r="S75" t="b">
-        <v>1</v>
-      </c>
-      <c r="T75">
-        <v>11856.551798592032</v>
-      </c>
-      <c r="U75" t="b">
-        <v>1</v>
-      </c>
-      <c r="V75">
-        <v>3</v>
-      </c>
-      <c r="W75">
-        <v>27</v>
-      </c>
-      <c r="X75">
-        <v>1</v>
-      </c>
-      <c r="Y75">
-        <v>66.366897583007813</v>
-      </c>
-      <c r="Z75" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA75" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB75" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC75" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD75" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>96</v>
-      </c>
-      <c r="B76" t="s">
-        <v>66</v>
-      </c>
-      <c r="C76" t="s">
-        <v>88</v>
-      </c>
-      <c r="D76" t="s">
-        <v>45</v>
-      </c>
-      <c r="E76" t="s">
-        <v>46</v>
-      </c>
-      <c r="F76" t="s">
-        <v>47</v>
-      </c>
-      <c r="G76" t="s">
-        <v>11</v>
-      </c>
-      <c r="H76" t="s">
-        <v>11</v>
-      </c>
-      <c r="I76" t="s">
-        <v>11</v>
-      </c>
-      <c r="J76" t="s">
-        <v>62</v>
-      </c>
-      <c r="K76" t="s">
-        <v>11</v>
-      </c>
-      <c r="L76" t="s">
-        <v>11</v>
-      </c>
-      <c r="M76" t="s">
-        <v>11</v>
-      </c>
-      <c r="N76" t="s">
-        <v>11</v>
-      </c>
-      <c r="O76" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P76" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>11</v>
-      </c>
-      <c r="R76" t="s">
-        <v>11</v>
-      </c>
-      <c r="S76" t="b">
-        <v>1</v>
-      </c>
-      <c r="T76">
-        <v>2446.3801850145992</v>
-      </c>
-      <c r="U76" t="b">
-        <v>1</v>
-      </c>
-      <c r="V76">
-        <v>3</v>
-      </c>
-      <c r="W76">
-        <v>18</v>
-      </c>
-      <c r="X76">
-        <v>1</v>
-      </c>
-      <c r="Y76">
-        <v>65.969253540039063</v>
-      </c>
-      <c r="Z76" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA76" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB76" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC76" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD76" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>106</v>
-      </c>
-      <c r="B77" t="s">
-        <v>66</v>
-      </c>
-      <c r="C77" t="s">
-        <v>98</v>
-      </c>
-      <c r="D77" t="s">
-        <v>45</v>
-      </c>
-      <c r="E77" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" t="s">
-        <v>47</v>
-      </c>
-      <c r="G77" t="s">
-        <v>11</v>
-      </c>
-      <c r="H77" t="s">
-        <v>11</v>
-      </c>
-      <c r="I77" t="s">
-        <v>11</v>
-      </c>
-      <c r="J77" t="s">
-        <v>62</v>
-      </c>
-      <c r="K77" t="s">
-        <v>11</v>
-      </c>
-      <c r="L77" t="s">
-        <v>11</v>
-      </c>
-      <c r="M77" t="s">
-        <v>11</v>
-      </c>
-      <c r="N77" t="s">
-        <v>11</v>
-      </c>
-      <c r="O77" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P77" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>11</v>
-      </c>
-      <c r="R77" t="s">
-        <v>11</v>
-      </c>
-      <c r="S77" t="b">
-        <v>1</v>
-      </c>
-      <c r="T77">
-        <v>453.9028514530811</v>
-      </c>
-      <c r="U77" t="b">
-        <v>1</v>
-      </c>
-      <c r="V77">
-        <v>3</v>
-      </c>
-      <c r="W77">
-        <v>39</v>
-      </c>
-      <c r="X77">
-        <v>1</v>
-      </c>
-      <c r="Y77">
-        <v>87.044357299804688</v>
-      </c>
-      <c r="Z77" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA77" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB77" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC77" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD77" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>116</v>
-      </c>
-      <c r="B78" t="s">
-        <v>66</v>
-      </c>
-      <c r="C78" t="s">
-        <v>108</v>
-      </c>
-      <c r="D78" t="s">
-        <v>45</v>
-      </c>
-      <c r="E78" t="s">
-        <v>46</v>
-      </c>
-      <c r="F78" t="s">
-        <v>47</v>
-      </c>
-      <c r="G78" t="s">
-        <v>11</v>
-      </c>
-      <c r="H78" t="s">
-        <v>11</v>
-      </c>
-      <c r="I78" t="s">
-        <v>11</v>
-      </c>
-      <c r="J78" t="s">
-        <v>62</v>
-      </c>
-      <c r="K78" t="s">
-        <v>11</v>
-      </c>
-      <c r="L78" t="s">
-        <v>11</v>
-      </c>
-      <c r="M78" t="s">
-        <v>11</v>
-      </c>
-      <c r="N78" t="s">
-        <v>11</v>
-      </c>
-      <c r="O78" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P78" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>11</v>
-      </c>
-      <c r="R78" t="s">
-        <v>11</v>
-      </c>
-      <c r="S78" t="b">
-        <v>1</v>
-      </c>
-      <c r="T78">
-        <v>949.45575971407459</v>
-      </c>
-      <c r="U78" t="b">
-        <v>1</v>
-      </c>
-      <c r="V78">
-        <v>3</v>
-      </c>
-      <c r="W78">
-        <v>9</v>
-      </c>
-      <c r="X78">
-        <v>1</v>
-      </c>
-      <c r="Y78">
-        <v>66.764541625976563</v>
-      </c>
-      <c r="Z78" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA78" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB78" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC78" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD78" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" t="s">
-        <v>66</v>
-      </c>
-      <c r="C79" t="s">
-        <v>118</v>
-      </c>
-      <c r="D79" t="s">
-        <v>45</v>
-      </c>
-      <c r="E79" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" t="s">
-        <v>47</v>
-      </c>
-      <c r="G79" t="s">
-        <v>11</v>
-      </c>
-      <c r="H79" t="s">
-        <v>11</v>
-      </c>
-      <c r="I79" t="s">
-        <v>11</v>
-      </c>
-      <c r="J79" t="s">
-        <v>62</v>
-      </c>
-      <c r="K79" t="s">
-        <v>11</v>
-      </c>
-      <c r="L79" t="s">
-        <v>11</v>
-      </c>
-      <c r="M79" t="s">
-        <v>11</v>
-      </c>
-      <c r="N79" t="s">
-        <v>11</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P79" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>11</v>
-      </c>
-      <c r="R79" t="s">
-        <v>11</v>
-      </c>
-      <c r="S79" t="b">
-        <v>1</v>
-      </c>
-      <c r="T79">
-        <v>8859.4800092846945</v>
-      </c>
-      <c r="U79" t="b">
-        <v>1</v>
-      </c>
-      <c r="V79">
-        <v>3</v>
-      </c>
-      <c r="W79">
-        <v>21</v>
-      </c>
-      <c r="X79">
-        <v>1</v>
-      </c>
-      <c r="Y79">
-        <v>64.179855346679688</v>
-      </c>
-      <c r="Z79" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA79" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB79" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC79" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD79" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>136</v>
-      </c>
-      <c r="B80" t="s">
-        <v>66</v>
-      </c>
-      <c r="C80" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" t="s">
-        <v>45</v>
-      </c>
-      <c r="E80" t="s">
-        <v>46</v>
-      </c>
-      <c r="F80" t="s">
-        <v>47</v>
-      </c>
-      <c r="G80" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" t="s">
-        <v>11</v>
-      </c>
-      <c r="I80" t="s">
-        <v>11</v>
-      </c>
-      <c r="J80" t="s">
-        <v>62</v>
-      </c>
-      <c r="K80" t="s">
-        <v>11</v>
-      </c>
-      <c r="L80" t="s">
-        <v>11</v>
-      </c>
-      <c r="M80" t="s">
-        <v>11</v>
-      </c>
-      <c r="N80" t="s">
-        <v>11</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P80" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>11</v>
-      </c>
-      <c r="R80" t="s">
-        <v>11</v>
-      </c>
-      <c r="S80" t="b">
-        <v>1</v>
-      </c>
-      <c r="T80">
-        <v>20991.264453125001</v>
-      </c>
-      <c r="U80" t="b">
-        <v>1</v>
-      </c>
-      <c r="V80">
-        <v>3</v>
-      </c>
-      <c r="W80">
-        <v>29</v>
-      </c>
-      <c r="X80">
-        <v>1</v>
-      </c>
-      <c r="Y80">
-        <v>85.056137084960938</v>
-      </c>
-      <c r="Z80">
-        <v>73.723297119140625</v>
-      </c>
-      <c r="AA80">
-        <v>60.998706817626953</v>
-      </c>
-      <c r="AB80" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC80" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD80" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>137</v>
-      </c>
-      <c r="B82" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>139</v>
-      </c>
-      <c r="B83" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>140</v>
-      </c>
-      <c r="B84" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>142</v>
-      </c>
-      <c r="B85" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>